<commit_message>
bead catalog parses in octave
</commit_message>
<xml_diff>
--- a/code/BeadCatalog.xlsx
+++ b/code/BeadCatalog.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="25600" windowHeight="15920" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="1700" windowWidth="26560" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,9 +32,96 @@
     <t>SpheroTech RCP-30-5A</t>
   </si>
   <si>
+    <t>(8 peaks), but not all are used in most channels since the lowest are not given MESF values in the tech notes</t>
+  </si>
+  <si>
+    <t>Lot AA01, AA02, AA03, AA04, AB01, AB02, AC01, GAA01-R</t>
+  </si>
+  <si>
     <t>FITC</t>
   </si>
   <si>
+    <t>530/40</t>
+  </si>
+  <si>
+    <t>MEFL</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>575/25</t>
+  </si>
+  <si>
+    <t>MEPE</t>
+  </si>
+  <si>
+    <t>PE-TR</t>
+  </si>
+  <si>
+    <t>613/20</t>
+  </si>
+  <si>
+    <t>MEPTR</t>
+  </si>
+  <si>
+    <t>PE-Cy5</t>
+  </si>
+  <si>
+    <t>680/30</t>
+  </si>
+  <si>
+    <t>MECY</t>
+  </si>
+  <si>
+    <t>PE-Cy7</t>
+  </si>
+  <si>
+    <t>750LP</t>
+  </si>
+  <si>
+    <t>MEPCY7</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>665/20</t>
+  </si>
+  <si>
+    <t>MEAP</t>
+  </si>
+  <si>
+    <t>APC-Cy7</t>
+  </si>
+  <si>
+    <t>MEAPCY7</t>
+  </si>
+  <si>
+    <t>Lot AC02, AC03, AD01</t>
+  </si>
+  <si>
+    <t>Lot AD04, AE01, AF01, AF02, AH01, AH02, AJ01</t>
+  </si>
+  <si>
+    <t>Lot AG01</t>
+  </si>
+  <si>
+    <t>Lot Z02, Z03</t>
+  </si>
+  <si>
+    <t>SpheroTech RCP-30-5</t>
+  </si>
+  <si>
+    <t>(6 peaks), but not all are used in most channels since the lowest are not given MESF values in the tech notes</t>
+  </si>
+  <si>
+    <t>Lot AA01, AB01, AB02, AC01, AD01</t>
+  </si>
+  <si>
+    <t>Lot AD03, AF01, AG01</t>
+  </si>
+  <si>
     <t>Clontech AcGFP 632594</t>
   </si>
   <si>
@@ -44,187 +131,100 @@
     <t>AcGFP/EGFP</t>
   </si>
   <si>
+    <t>MESF</t>
+  </si>
+  <si>
     <t>Clontech mCherry 632595</t>
   </si>
   <si>
+    <t>Also called TaKaRa mCherry</t>
+  </si>
+  <si>
+    <t>Lot 1308012</t>
+  </si>
+  <si>
     <t>mCherry</t>
   </si>
   <si>
-    <t>Lot 1308012</t>
-  </si>
-  <si>
-    <t>Also called TaKaRa mCherry</t>
-  </si>
-  <si>
     <t>Lot 1612008</t>
   </si>
   <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>PE-TR</t>
-  </si>
-  <si>
-    <t>PE-Cy5</t>
-  </si>
-  <si>
-    <t>PE-Cy7</t>
-  </si>
-  <si>
-    <t>APC</t>
-  </si>
-  <si>
-    <t>APC-Cy7</t>
-  </si>
-  <si>
-    <t>750LP</t>
-  </si>
-  <si>
-    <t>665/20</t>
-  </si>
-  <si>
-    <t>680/30</t>
-  </si>
-  <si>
-    <t>613/20</t>
-  </si>
-  <si>
-    <t>530/40</t>
-  </si>
-  <si>
-    <t>Lot AC02, AC03, AD01</t>
-  </si>
-  <si>
-    <t>Lot AA01, AA02, AA03, AA04, AB01, AB02, AC01, GAA01-R</t>
-  </si>
-  <si>
-    <t>Lot AG01</t>
-  </si>
-  <si>
-    <t>Lot Z02, Z03</t>
-  </si>
-  <si>
-    <t>(8 peaks), but not all are used in most channels since the lowest are not given MESF values in the tech notes</t>
-  </si>
-  <si>
-    <t>SpheroTech RCP-30-5</t>
-  </si>
-  <si>
-    <t>(6 peaks), but not all are used in most channels since the lowest are not given MESF values in the tech notes</t>
-  </si>
-  <si>
-    <t>Lot AA01, AB01, AB02, AC01, AD01</t>
-  </si>
-  <si>
-    <t>Lot AD03, AF01, AG01</t>
-  </si>
-  <si>
-    <t>MEFL</t>
-  </si>
-  <si>
-    <t>MEPE</t>
-  </si>
-  <si>
-    <t>MEPTR</t>
-  </si>
-  <si>
-    <t>MECY</t>
-  </si>
-  <si>
-    <t>MEAP</t>
-  </si>
-  <si>
-    <t>MEPCY7</t>
-  </si>
-  <si>
-    <t>MEAPCY7</t>
-  </si>
-  <si>
-    <t>MESF</t>
-  </si>
-  <si>
-    <t>Lot AD04, AE01, AF01, AF02, AH01, AH02, AJ01</t>
-  </si>
-  <si>
     <t>SpheroTech URCP-38-2K</t>
   </si>
   <si>
+    <t>(6 peaks), Rev E/F uses newer F values in case of conflict</t>
+  </si>
+  <si>
+    <t>Rev E/F</t>
+  </si>
+  <si>
+    <t>BV421</t>
+  </si>
+  <si>
+    <t>450/50</t>
+  </si>
+  <si>
     <t>MEBV421</t>
   </si>
   <si>
+    <t>BV500</t>
+  </si>
+  <si>
+    <t>525/50</t>
+  </si>
+  <si>
     <t>MEBV500</t>
   </si>
   <si>
+    <t>BV605</t>
+  </si>
+  <si>
+    <t>610/20</t>
+  </si>
+  <si>
     <t>MEBV605</t>
   </si>
   <si>
     <t>MEPCY5</t>
   </si>
   <si>
+    <t>PerCP</t>
+  </si>
+  <si>
+    <t>710/50</t>
+  </si>
+  <si>
     <t>MEPerCP</t>
   </si>
   <si>
-    <t>BV421</t>
-  </si>
-  <si>
-    <t>BV500</t>
-  </si>
-  <si>
-    <t>BV605</t>
-  </si>
-  <si>
-    <t>PerCP</t>
-  </si>
-  <si>
     <t>PerCP-Cy5.5</t>
   </si>
   <si>
+    <t>695/40</t>
+  </si>
+  <si>
     <t>MEPerCPCy5.5</t>
   </si>
   <si>
     <t>APC-R700</t>
   </si>
   <si>
+    <t>730/45</t>
+  </si>
+  <si>
     <t>MER700</t>
   </si>
   <si>
-    <t>450/50</t>
-  </si>
-  <si>
-    <t>525/50</t>
-  </si>
-  <si>
-    <t>610/20</t>
-  </si>
-  <si>
-    <t>710/50</t>
-  </si>
-  <si>
-    <t>695/40</t>
-  </si>
-  <si>
-    <t>730/45</t>
-  </si>
-  <si>
     <t>Cascade Blue</t>
   </si>
   <si>
+    <t>MECSB</t>
+  </si>
+  <si>
     <t>BFP</t>
   </si>
   <si>
     <t>MEBFP</t>
-  </si>
-  <si>
-    <t>MECSB</t>
-  </si>
-  <si>
-    <t>Rev E/F</t>
-  </si>
-  <si>
-    <t>(6 peaks), Rev E/F uses newer F values in case of conflict</t>
-  </si>
-  <si>
-    <t>575/25</t>
   </si>
 </sst>
 </file>
@@ -262,8 +262,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -272,7 +272,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -292,44 +292,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -359,12 +359,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -403,246 +403,178 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>488</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>692</v>
@@ -665,27 +597,19 @@
       <c r="M2">
         <v>291016</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>488</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>505</v>
@@ -709,18 +633,18 @@
         <v>250485</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>488</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4">
-        <v>488</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
       </c>
       <c r="G4">
         <v>207</v>
@@ -744,7 +668,7 @@
         <v>170258</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -752,10 +676,10 @@
         <v>488</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>1437</v>
@@ -778,17 +702,10 @@
       <c r="M5">
         <v>1069885</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>488</v>
@@ -797,7 +714,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="K6">
         <v>32907</v>
@@ -809,18 +726,18 @@
         <v>503798</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>635</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>578</v>
@@ -844,9 +761,9 @@
         <v>146090</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>635</v>
@@ -855,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>718</v>
@@ -876,124 +793,124 @@
         <v>26735</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>488</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
         <v>91.287655108579187</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>682.22958580181671</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>2169.7268723424163</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>5987.5729116689954</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>18187.295867266253</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>37095.973305539745</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <v>127454.3853277982</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>293312.93284753093</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>488</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>59.844766849088266</v>
+      </c>
+      <c r="G10" s="1">
+        <v>516.15719933716571</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1781.3518196666203</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4981.5086938794921</v>
+      </c>
+      <c r="J10" s="1">
+        <v>13434.851540821801</v>
+      </c>
+      <c r="K10" s="1">
+        <v>27135.661548356544</v>
+      </c>
+      <c r="L10" s="1">
+        <v>96204.61409778634</v>
+      </c>
+      <c r="M10" s="1">
+        <v>259412.61657136423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>488</v>
+      </c>
+      <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
-        <v>488</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="2">
-        <v>59.844766849088266</v>
-      </c>
-      <c r="G10" s="2">
-        <v>516.15719933716571</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1781.3518196666203</v>
-      </c>
-      <c r="I10" s="2">
-        <v>4981.5086938794921</v>
-      </c>
-      <c r="J10" s="2">
-        <v>13434.851540821801</v>
-      </c>
-      <c r="K10" s="2">
-        <v>27135.661548356544</v>
-      </c>
-      <c r="L10" s="2">
-        <v>96204.61409778634</v>
-      </c>
-      <c r="M10" s="2">
-        <v>259412.61657136423</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
-        <v>488</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>20.990600181712118</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>218.12305864236004</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>737.20668907733102</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>2197.5712924899599</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>6081.9597418204967</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>13048.069133703204</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>52446.889131816963</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <v>177982.88390737993</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1001,39 +918,39 @@
         <v>488</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="2">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1">
         <v>252.04366804505688</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>1434.9834237807906</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>4725.1255293937247</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>12977.457908451384</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>34975.098613213457</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>71893.29906907001</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>258366.2153671055</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>1120607.1114736947</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>488</v>
@@ -1042,62 +959,62 @@
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="2">
+        <v>17</v>
+      </c>
+      <c r="J13" s="1">
         <v>14808.287226012746</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>31811.505501680942</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <v>105241.06701062211</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <v>523450.79639630229</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>635</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="2">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
         <v>190.61467429802846</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>1147.002774943423</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>4022.2723284442973</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>9252.2079612463003</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>21224.727541324479</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>36065.432938049496</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <v>61473.156829862157</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <v>155931.99695048877</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>635</v>
@@ -1106,138 +1023,138 @@
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="2">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1">
         <v>1638.4451791114259</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <v>4232.8797003199934</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <v>8021.7436831980385</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="1">
         <v>14091.806034238376</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="1">
         <v>27002.385013650975</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>488</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
         <v>90.708688638215349</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>791.21979760346414</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>2083.0123488325257</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>6561.8826258388208</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>16530.738141233476</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>47575.3135266221</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <v>136680.14281623816</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="1">
         <v>271771.18947984645</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>488</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="2">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
         <v>58.504591870998077</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>529.18591069875038</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>1512.780201818656</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>4820.1566358577466</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>12482.788559073864</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>36107.548901544993</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <v>109419.83713995016</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
         <v>251439.20289082278</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>488</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="C18">
-        <v>488</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>21.421468649462536</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>233.84314642996344</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>662.84032195643624</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>2183.3868785304467</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>5945.5319801879732</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <v>18292.089005332233</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <v>63953.948585701495</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="1">
         <v>188159.82006959253</v>
       </c>
     </row>
@@ -1249,39 +1166,39 @@
         <v>488</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1">
         <v>223.52150025935381</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>1643.8118144687353</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
         <v>3981.320869465118</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <v>11941.344333110494</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>31772.979705440648</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>95618.694126656526</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="1">
         <v>354172.14762356674</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="1">
         <v>1081652.6875898393</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>488</v>
@@ -1290,66 +1207,66 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1">
         <v>14916.456985033405</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>42336.49643025847</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="1">
         <v>153840.44272368916</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="1">
         <v>494262.78101307119</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>635</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="2">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1">
         <v>33.059289385083844</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>384.30527062164651</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>1047.7271905090386</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <v>3617.5569258322357</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="1">
         <v>9826.3433909565101</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>28203.748047323141</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="1">
         <v>80107.936436489123</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="1">
         <v>152052.06356548588</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>635</v>
@@ -1358,139 +1275,139 @@
         <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1">
         <v>2863.8652997650343</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>7644.4004782779293</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="1">
         <v>19081.426772660452</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="1">
         <v>37257.741435713819</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>488</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1">
         <v>72.118664154335406</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>645.65082125628419</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>1704.676894021791</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="1">
         <v>4828.1663767473601</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="1">
         <v>15994.701295388273</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>47601.851041699985</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="1">
         <v>135873.44304252969</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="1">
         <v>273002.35313998547</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>488</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="2">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1">
         <v>61.810389305459346</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>418.06637177187042</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>1187.9904177960275</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>3444.7795138031493</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="1">
         <v>11855.152867326651</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>35820.903138309302</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="1">
         <v>108155.00029853273</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="1">
         <v>248049.25900143688</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>488</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
         <v>11</v>
       </c>
-      <c r="C25">
-        <v>488</v>
-      </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>18.605159209039591</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>181.83239875676099</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>512.42282060717514</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>1503.426353368227</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <v>5542.9085827056733</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>17660.773523144086</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="1">
         <v>61832.518666543576</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <v>179698.3543498595</v>
       </c>
     </row>
@@ -1502,39 +1419,39 @@
         <v>488</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="2">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1">
         <v>211.94708634426496</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>1300.8094530223825</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>3259.8232710967163</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <v>8682.988333529107</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="1">
         <v>30544.249082178543</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="1">
         <v>94729.607621595394</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="1">
         <v>355084.50877872051</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="1">
         <v>1041298.2660207922</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27">
         <v>488</v>
@@ -1543,64 +1460,64 @@
         <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1">
         <v>44126.509434228574</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="1">
         <v>153458.00307923602</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="1">
         <v>477991.44006706</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C28">
         <v>635</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="2">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1">
         <v>22.39555129947307</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>292.03676769721244</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>902.71536120103713</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <v>2944.5960137322199</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="1">
         <v>10278.80453033005</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1">
         <v>31831.416224035762</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="1">
         <v>88782.266542445024</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="1">
         <v>136879.68660749335</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C29">
         <v>635</v>
@@ -1609,138 +1526,138 @@
         <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="2">
+        <v>22</v>
+      </c>
+      <c r="F29" s="1">
         <v>25.928570482017061</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>152.48101051263112</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>358.00436564992799</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <v>966.61177225836548</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <v>2861.6509302587574</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>8041.5025813742322</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="1">
         <v>21487.945825907238</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="1">
         <v>34373.149263290208</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>488</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="1">
         <v>600.35775263131416</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>1644.8836052516158</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <v>4922.4424702230008</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="1">
         <v>15195.881971248607</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="1">
         <v>39662.706721527851</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="1">
         <v>149665.84397616773</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="1">
         <v>309755.21324948978</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C31">
         <v>488</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="2">
+        <v>8</v>
+      </c>
+      <c r="G31" s="1">
         <v>404.10533494377052</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
         <v>1095.6167947520034</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <v>3753.0293577842062</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="1">
         <v>11969.108480750741</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1">
         <v>29594.191377623931</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="1">
         <v>126938.09421747926</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="1">
         <v>292771.28196029278</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>488</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
         <v>11</v>
       </c>
-      <c r="C32">
-        <v>488</v>
-      </c>
-      <c r="D32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>174.9385848698565</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>479.7049082410262</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>1686.8511742460757</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
         <v>5559.6438157523389</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>14005.987867663736</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="1">
         <v>66196.55500198713</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="1">
         <v>180682.43671634301</v>
       </c>
     </row>
@@ -1752,175 +1669,175 @@
         <v>488</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="2">
+        <v>14</v>
+      </c>
+      <c r="G33" s="1">
         <v>1685.5047268701346</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
         <v>3599.9570948625665</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="1">
         <v>10444.988860867094</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
         <v>29718.586839232412</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="1">
         <v>70128.18193844505</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="1">
         <v>310592.89779807127</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="1">
         <v>830795.86465867609</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C34">
         <v>635</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2">
+        <v>20</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
         <v>6560.3133791414384</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>11080.766809312474</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>20692.124966656658</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="1">
         <v>67896.246681437377</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="1">
         <v>133802.14051552708</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>488</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="2">
+        <v>5</v>
+      </c>
+      <c r="G37" s="1">
         <v>6028.199445412838</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="1">
         <v>17492.24021196477</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="1">
         <v>35673.850921381425</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="1">
         <v>126907.40070512844</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="1">
         <v>290986.30857787863</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C38">
         <v>488</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="2">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1">
         <v>4973.9746892077674</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="1">
         <v>13117.893597155413</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="1">
         <v>26757.541803125387</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="1">
         <v>94929.860964850042</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="1">
         <v>250468.6012952716</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>488</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
         <v>11</v>
       </c>
-      <c r="C39">
-        <v>488</v>
-      </c>
-      <c r="D39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>2198.0605867523991</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="1">
         <v>6062.7099224220547</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="1">
         <v>12887.164902927385</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="1">
         <v>51686.288153170259</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="1">
         <v>170219.32510029379</v>
       </c>
     </row>
@@ -1932,150 +1849,150 @@
         <v>488</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2">
+        <v>14</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1">
         <v>36838.560009079178</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="1">
         <v>76620.919524591824</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="1">
         <v>261645.00925298303</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="1">
         <v>1069920.0890999043</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>635</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" s="2">
+        <v>20</v>
+      </c>
+      <c r="G41" s="1">
         <v>6921.8384433726742</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>17529.728659174853</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="1">
         <v>29733.561033593178</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="1">
         <v>52783.806132992286</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="1">
         <v>147766.14355347541</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>488</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="2">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1">
         <v>58.40904585895818</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>4817.5993491501431</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>16087.353969081689</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="1">
         <v>34482.847193571622</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="1">
         <v>127381.84724128884</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="1">
         <v>319240.8573756913</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>488</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43" s="2">
+        <v>8</v>
+      </c>
+      <c r="F43" s="1">
         <v>14.150709353130571</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>3906.3406571983301</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="1">
         <v>11164.166669288212</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="1">
         <v>24667.207339539553</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="1">
         <v>97369.548586795005</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="1">
         <v>297396.34113562782</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>488</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
         <v>11</v>
       </c>
-      <c r="C44">
-        <v>488</v>
-      </c>
-      <c r="D44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" t="s">
-        <v>32</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>3.4068990350046349</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
         <v>1699.318755795259</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="1">
         <v>5424.162581403607</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="1">
         <v>13027.605241080961</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="1">
         <v>59419.766398513842</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1">
         <v>204118.4615559896</v>
       </c>
     </row>
@@ -2087,33 +2004,33 @@
         <v>488</v>
       </c>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="2">
+        <v>14</v>
+      </c>
+      <c r="F45" s="1">
         <v>69.97518586568799</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>10543.285640832099</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="1">
         <v>30840.184416983655</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="1">
         <v>69203.593696684751</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="1">
         <v>268757.08137686923</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>1308307.6819744271</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C46">
         <v>488</v>
@@ -2122,62 +2039,62 @@
         <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" s="2">
+        <v>17</v>
+      </c>
+      <c r="F46" s="1">
         <v>121.88334626289472</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
         <v>4447.5297743121182</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="1">
         <v>12826.634410073089</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="1">
         <v>41676.365575392017</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="1">
         <v>149440.70141869233</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="1">
         <v>474797.25239198504</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C47">
         <v>635</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="2">
+        <v>20</v>
+      </c>
+      <c r="F47" s="1">
         <v>8.3799739194058205</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
         <v>2677.3289624840249</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="1">
         <v>9858.3768981945341</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="1">
         <v>22058.029216762705</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="1">
         <v>51843.957956180602</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="1">
         <v>199751.06578643262</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C48">
         <v>635</v>
@@ -2186,59 +2103,59 @@
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="2">
+        <v>22</v>
+      </c>
+      <c r="F48" s="1">
         <v>1.342642981549361</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
         <v>503.99023086982908</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="1">
         <v>2252.3865973543079</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="1">
         <v>5985.1151786170622</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48" s="1">
         <v>13616.659584949804</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="1">
         <v>40093.000181074385</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>2</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C51">
         <v>488</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F51">
         <v>74471</v>
@@ -2261,24 +2178,24 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C54">
         <v>561</v>
       </c>
       <c r="E54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F54">
         <v>521</v>
@@ -2301,16 +2218,16 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C55">
         <v>561</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F55">
         <v>3616</v>
@@ -2333,27 +2250,27 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>488</v>
       </c>
       <c r="D58" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G58">
         <v>2615</v>
@@ -2373,16 +2290,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C59">
         <v>488</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="G59">
         <v>2205</v>
@@ -2408,10 +2325,10 @@
         <v>488</v>
       </c>
       <c r="D60" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G60">
         <v>1270</v>
@@ -2431,16 +2348,16 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C61">
         <v>635</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G61">
         <v>6780</v>
@@ -2460,19 +2377,19 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C62">
         <v>405</v>
       </c>
       <c r="D62" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F62" s="3">
         <v>48.660152022096099</v>
@@ -2501,42 +2418,42 @@
         <v>405</v>
       </c>
       <c r="D63" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E63" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="2">
+        <v>48</v>
+      </c>
+      <c r="F63" s="1">
         <v>891.46977890254573</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
         <v>1749.3288885509437</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63" s="1">
         <v>6322.9330653897014</v>
       </c>
-      <c r="I63" s="2">
+      <c r="I63" s="1">
         <v>13158.048052157212</v>
       </c>
-      <c r="J63" s="2">
+      <c r="J63" s="1">
         <v>28040.039078716985</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="1">
         <v>52698.477020820304</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C64">
         <v>405</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E64" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F64" s="3">
         <v>1331.5136151464262</v>
@@ -2559,16 +2476,16 @@
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>488</v>
       </c>
       <c r="D65" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F65" s="3">
         <v>154.29662243076513</v>
@@ -2591,16 +2508,16 @@
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C66">
         <v>488</v>
       </c>
       <c r="D66" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="F66" s="3">
         <v>94.109451178046356</v>
@@ -2623,16 +2540,16 @@
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>488</v>
+      </c>
+      <c r="D67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
         <v>11</v>
-      </c>
-      <c r="C67">
-        <v>488</v>
-      </c>
-      <c r="D67" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" t="s">
-        <v>32</v>
       </c>
       <c r="F67" s="3">
         <v>317.96520504415537</v>
@@ -2661,10 +2578,10 @@
         <v>488</v>
       </c>
       <c r="D68" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E68" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F68" s="3">
         <v>32.017831087730912</v>
@@ -2687,16 +2604,16 @@
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C69">
         <v>488</v>
       </c>
       <c r="D69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E69" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F69" s="3">
         <v>417.42372721643846</v>
@@ -2719,7 +2636,7 @@
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C70">
         <v>560</v>
@@ -2728,7 +2645,7 @@
         <v>57</v>
       </c>
       <c r="E70" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F70" s="3">
         <v>46.599869524605857</v>
@@ -2751,7 +2668,7 @@
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C71">
         <v>488</v>
@@ -2760,7 +2677,7 @@
         <v>16</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="F71" s="3">
         <v>29.866627546433204</v>
@@ -2783,16 +2700,16 @@
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C72">
         <v>633</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E72" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F72" s="3">
         <v>226.37632089238281</v>
@@ -2815,16 +2732,16 @@
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C73">
         <v>633</v>
       </c>
       <c r="D73" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F73" s="3">
         <v>18.071891640667513</v>
@@ -2847,7 +2764,7 @@
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C74">
         <v>635</v>
@@ -2856,7 +2773,7 @@
         <v>16</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F74" s="3">
         <v>4.4699214631866608</v>
@@ -2879,70 +2796,69 @@
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C75">
         <v>405</v>
       </c>
       <c r="D75" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E75" t="s">
-        <v>62</v>
-      </c>
-      <c r="F75" s="2">
+        <v>63</v>
+      </c>
+      <c r="F75" s="1">
         <v>100.73924657524458</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75" s="1">
         <v>211.17373388135246</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75" s="1">
         <v>1267.9817745439038</v>
       </c>
-      <c r="I75" s="2">
+      <c r="I75" s="1">
         <v>3498.4007571732591</v>
       </c>
-      <c r="J75" s="2">
+      <c r="J75" s="1">
         <v>8965.0896474047058</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="1">
         <v>20695.114194178357</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C76">
         <v>405</v>
       </c>
       <c r="D76" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>61</v>
-      </c>
-      <c r="F76" s="2">
+        <v>65</v>
+      </c>
+      <c r="F76" s="1">
         <v>184.88733756527577</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G76" s="1">
         <v>608.05492599895808</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76" s="1">
         <v>4103.6058068986968</v>
       </c>
-      <c r="I76" s="2">
+      <c r="I76" s="1">
         <v>11560.019375163876</v>
       </c>
-      <c r="J76" s="2">
+      <c r="J76" s="1">
         <v>30734.983150983873</v>
       </c>
-      <c r="K76" s="2">
+      <c r="K76" s="1">
         <v>72372.592439871049</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bead lot AJ02 added
</commit_message>
<xml_diff>
--- a/code/BeadCatalog.xlsx
+++ b/code/BeadCatalog.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/code/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1700" windowWidth="26560" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="9680" yWindow="2080" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -225,18 +220,91 @@
   </si>
   <si>
     <t>MEBFP</t>
+  </si>
+  <si>
+    <t>Lot AJ02</t>
+  </si>
+  <si>
+    <t>MEBV510</t>
+  </si>
+  <si>
+    <t>MEBV650</t>
+  </si>
+  <si>
+    <t>MEBV711</t>
+  </si>
+  <si>
+    <t>MEBV786</t>
+  </si>
+  <si>
+    <t>MEPCY5.5</t>
+  </si>
+  <si>
+    <t>MEAlexa 700</t>
+  </si>
+  <si>
+    <t>MEBUV395</t>
+  </si>
+  <si>
+    <t>MEBUV737</t>
+  </si>
+  <si>
+    <t>BV510</t>
+  </si>
+  <si>
+    <t>BV650</t>
+  </si>
+  <si>
+    <t>BV711</t>
+  </si>
+  <si>
+    <t>BV786</t>
+  </si>
+  <si>
+    <t>ECD</t>
+  </si>
+  <si>
+    <t>PE-Cy5.5</t>
+  </si>
+  <si>
+    <t>Alexa 7000</t>
+  </si>
+  <si>
+    <t>BUV395</t>
+  </si>
+  <si>
+    <t>BUV737</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -257,8 +325,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -268,7 +346,17 @@
       <protection hidden="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -324,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -359,7 +447,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -536,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -544,15 +632,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N76"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N76"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -598,7 +689,7 @@
         <v>291016</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -633,7 +724,7 @@
         <v>250485</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -668,7 +759,7 @@
         <v>170258</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -703,7 +794,7 @@
         <v>1069885</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -726,7 +817,7 @@
         <v>503798</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -761,7 +852,7 @@
         <v>146090</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -793,7 +884,7 @@
         <v>26735</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -834,7 +925,7 @@
         <v>293312.93284753093</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -872,7 +963,7 @@
         <v>259412.61657136423</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -910,7 +1001,7 @@
         <v>177982.88390737993</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -948,7 +1039,7 @@
         <v>1120607.1114736947</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -974,7 +1065,7 @@
         <v>523450.79639630229</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1012,7 +1103,7 @@
         <v>155931.99695048877</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1132,7 @@
         <v>27002.385013650975</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1082,7 +1173,7 @@
         <v>271771.18947984645</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1120,7 +1211,7 @@
         <v>251439.20289082278</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1249,7 @@
         <v>188159.82006959253</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1196,7 +1287,7 @@
         <v>1081652.6875898393</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1226,7 +1317,7 @@
         <v>494262.78101307119</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -1264,7 +1355,7 @@
         <v>152052.06356548588</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1294,7 +1385,7 @@
         <v>37257.741435713819</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1426,7 @@
         <v>273002.35313998547</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1373,7 +1464,7 @@
         <v>248049.25900143688</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -1411,7 +1502,7 @@
         <v>179698.3543498595</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +1540,7 @@
         <v>1041298.2660207922</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="B27" t="s">
         <v>15</v>
       </c>
@@ -1477,7 +1568,7 @@
         <v>477991.44006706</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -1515,7 +1606,7 @@
         <v>136879.68660749335</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -1553,7 +1644,7 @@
         <v>34373.149263290208</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +1682,7 @@
         <v>309755.21324948978</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1626,7 +1717,7 @@
         <v>292771.28196029278</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1661,7 +1752,7 @@
         <v>180682.43671634301</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -1696,7 +1787,7 @@
         <v>830795.86465867609</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1727,7 +1818,7 @@
         <v>133802.14051552708</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1736,7 +1827,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1751,7 +1842,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1783,7 +1874,7 @@
         <v>290986.30857787863</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -1812,7 +1903,7 @@
         <v>250468.6012952716</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -1841,7 +1932,7 @@
         <v>170219.32510029379</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="B40" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1959,7 @@
         <v>1069920.0890999043</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -1897,7 +1988,7 @@
         <v>147766.14355347541</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1932,7 +2023,7 @@
         <v>319240.8573756913</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -1964,7 +2055,7 @@
         <v>297396.34113562782</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1996,7 +2087,7 @@
         <v>204118.4615559896</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="B45" t="s">
         <v>12</v>
       </c>
@@ -2028,7 +2119,7 @@
         <v>1308307.6819744271</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="B46" t="s">
         <v>15</v>
       </c>
@@ -2060,7 +2151,7 @@
         <v>474797.25239198504</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="B47" t="s">
         <v>18</v>
       </c>
@@ -2092,7 +2183,7 @@
         <v>199751.06578643262</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="B48" t="s">
         <v>21</v>
       </c>
@@ -2124,7 +2215,7 @@
         <v>40093.000181074385</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14">
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="K49" s="2"/>
@@ -2132,7 +2223,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2144,7 +2235,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -2176,7 +2267,7 @@
         <v>18463961</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -2184,7 +2275,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2216,7 +2307,7 @@
         <v>4309984</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -2248,7 +2339,7 @@
         <v>5947886</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>40</v>
       </c>
@@ -2256,7 +2347,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2288,7 +2379,7 @@
         <v>328880</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14">
       <c r="B59" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2408,7 @@
         <v>248895</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="B60" t="s">
         <v>12</v>
       </c>
@@ -2346,7 +2437,7 @@
         <v>618430</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14">
       <c r="B61" t="s">
         <v>18</v>
       </c>
@@ -2375,7 +2466,7 @@
         <v>919070</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2410,7 +2501,7 @@
         <v>20378.471643026176</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14">
       <c r="B63" t="s">
         <v>46</v>
       </c>
@@ -2442,7 +2533,7 @@
         <v>52698.477020820304</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14">
       <c r="B64" t="s">
         <v>49</v>
       </c>
@@ -2474,7 +2565,7 @@
         <v>159814.80526382173</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -2506,7 +2597,7 @@
         <v>450950.92072795785</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="B66" t="s">
         <v>6</v>
       </c>
@@ -2538,7 +2629,7 @@
         <v>317887.98611741111</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="B67" t="s">
         <v>9</v>
       </c>
@@ -2570,7 +2661,7 @@
         <v>1187118.7704526538</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="B68" t="s">
         <v>12</v>
       </c>
@@ -2602,7 +2693,7 @@
         <v>1115313.181575086</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="B69" t="s">
         <v>53</v>
       </c>
@@ -2634,7 +2725,7 @@
         <v>536053.21610669303</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="B70" t="s">
         <v>56</v>
       </c>
@@ -2666,7 +2757,7 @@
         <v>51747.05130671752</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="B71" t="s">
         <v>15</v>
       </c>
@@ -2698,7 +2789,7 @@
         <v>1267178.7601849632</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="B72" t="s">
         <v>18</v>
       </c>
@@ -2730,7 +2821,7 @@
         <v>104657.29839566484</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="B73" t="s">
         <v>59</v>
       </c>
@@ -2762,7 +2853,7 @@
         <v>1288085.751604842</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="B74" t="s">
         <v>21</v>
       </c>
@@ -2794,7 +2885,7 @@
         <v>260610.50236340964</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="B75" t="s">
         <v>62</v>
       </c>
@@ -2826,7 +2917,7 @@
         <v>20695.114194178357</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="B76" t="s">
         <v>64</v>
       </c>
@@ -2858,7 +2949,516 @@
         <v>72372.592439871049</v>
       </c>
     </row>
+    <row r="77" spans="1:11">
+      <c r="A77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E77" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="3">
+        <v>152</v>
+      </c>
+      <c r="G77" s="3">
+        <v>529</v>
+      </c>
+      <c r="H77" s="3">
+        <v>2416</v>
+      </c>
+      <c r="I77" s="3">
+        <v>5899</v>
+      </c>
+      <c r="J77" s="3">
+        <v>13266</v>
+      </c>
+      <c r="K77" s="3">
+        <v>26699</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="B78" t="s">
+        <v>75</v>
+      </c>
+      <c r="E78" t="s">
+        <v>67</v>
+      </c>
+      <c r="F78" s="1">
+        <v>439.03108723579822</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1128.1165738811235</v>
+      </c>
+      <c r="H78" s="1">
+        <v>5250.1626972944832</v>
+      </c>
+      <c r="I78" s="1">
+        <v>13404.439382284159</v>
+      </c>
+      <c r="J78" s="1">
+        <v>32187.960560894164</v>
+      </c>
+      <c r="K78" s="1">
+        <v>66013.697333474352</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="B79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="s">
+        <v>51</v>
+      </c>
+      <c r="F79" s="1">
+        <v>473.48120845241425</v>
+      </c>
+      <c r="G79" s="1">
+        <v>888.89247325914778</v>
+      </c>
+      <c r="H79" s="1">
+        <v>3308.2323795700468</v>
+      </c>
+      <c r="I79" s="1">
+        <v>8096.430093766975</v>
+      </c>
+      <c r="J79" s="1">
+        <v>21927.409708467672</v>
+      </c>
+      <c r="K79" s="1">
+        <v>63543.925886697034</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="B80" t="s">
+        <v>76</v>
+      </c>
+      <c r="E80" t="s">
+        <v>68</v>
+      </c>
+      <c r="F80" s="1">
+        <v>356.27932187382771</v>
+      </c>
+      <c r="G80" s="1">
+        <v>781.34482620455105</v>
+      </c>
+      <c r="H80" s="1">
+        <v>3000.9365772192568</v>
+      </c>
+      <c r="I80" s="1">
+        <v>7266.969156879848</v>
+      </c>
+      <c r="J80" s="1">
+        <v>20931.195845993956</v>
+      </c>
+      <c r="K80" s="1">
+        <v>62364.625703974802</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11">
+      <c r="B81" t="s">
+        <v>77</v>
+      </c>
+      <c r="E81" t="s">
+        <v>69</v>
+      </c>
+      <c r="F81" s="1">
+        <v>161.4064963311495</v>
+      </c>
+      <c r="G81" s="1">
+        <v>706.37121865124288</v>
+      </c>
+      <c r="H81" s="1">
+        <v>2806.2561765989694</v>
+      </c>
+      <c r="I81" s="1">
+        <v>6536.3741423501024</v>
+      </c>
+      <c r="J81" s="1">
+        <v>19293.055472706204</v>
+      </c>
+      <c r="K81" s="1">
+        <v>56753.374460214582</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11">
+      <c r="B82" t="s">
+        <v>78</v>
+      </c>
+      <c r="E82" t="s">
+        <v>70</v>
+      </c>
+      <c r="F82" s="1">
+        <v>152.00296959201486</v>
+      </c>
+      <c r="G82" s="1">
+        <v>706.74870229900523</v>
+      </c>
+      <c r="H82" s="1">
+        <v>2758.2310238877872</v>
+      </c>
+      <c r="I82" s="1">
+        <v>6388.9539650885108</v>
+      </c>
+      <c r="J82" s="1">
+        <v>19061.981025414228</v>
+      </c>
+      <c r="K82" s="1">
+        <v>56137.007707292629</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11">
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="1">
+        <v>190.37469148459621</v>
+      </c>
+      <c r="G83" s="1">
+        <v>3867.786255674208</v>
+      </c>
+      <c r="H83" s="1">
+        <v>33700.918610833403</v>
+      </c>
+      <c r="I83" s="1">
+        <v>97304.301498948014</v>
+      </c>
+      <c r="J83" s="1">
+        <v>251992.15196370424</v>
+      </c>
+      <c r="K83" s="1">
+        <v>485705.50301505951</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11">
+      <c r="B84" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F84" s="1">
+        <v>98.373492455450659</v>
+      </c>
+      <c r="G84" s="1">
+        <v>606.67301182136453</v>
+      </c>
+      <c r="H84" s="1">
+        <v>2986.1555651889935</v>
+      </c>
+      <c r="I84" s="1">
+        <v>7176.0739910682232</v>
+      </c>
+      <c r="J84" s="1">
+        <v>19997.042457093306</v>
+      </c>
+      <c r="K84" s="1">
+        <v>55123.971224972251</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11">
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="1">
+        <v>202.29113376298974</v>
+      </c>
+      <c r="G85" s="1">
+        <v>3041.3914157579152</v>
+      </c>
+      <c r="H85" s="1">
+        <v>25416.732533159342</v>
+      </c>
+      <c r="I85" s="1">
+        <v>72565.671201345162</v>
+      </c>
+      <c r="J85" s="1">
+        <v>182449.44318798327</v>
+      </c>
+      <c r="K85" s="1">
+        <v>337422.97853423643</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11">
+      <c r="B86" t="s">
+        <v>79</v>
+      </c>
+      <c r="E86" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="1">
+        <v>9.8194131263984676</v>
+      </c>
+      <c r="G86" s="1">
+        <v>6604.493123628401</v>
+      </c>
+      <c r="H86" s="1">
+        <v>61317.026926697305</v>
+      </c>
+      <c r="I86" s="1">
+        <v>183370.75879826702</v>
+      </c>
+      <c r="J86" s="1">
+        <v>492055.089919544</v>
+      </c>
+      <c r="K86" s="1">
+        <v>1027045.343192119</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11">
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87">
+        <v>488</v>
+      </c>
+      <c r="E87" t="s">
+        <v>52</v>
+      </c>
+      <c r="F87" s="1">
+        <v>66.18703784592276</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1210.7095889196451</v>
+      </c>
+      <c r="H87" s="1">
+        <v>15491.726172542774</v>
+      </c>
+      <c r="I87" s="1">
+        <v>62603.418084031873</v>
+      </c>
+      <c r="J87" s="1">
+        <v>298933.37238125486</v>
+      </c>
+      <c r="K87" s="1">
+        <v>1320053.0432920777</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11">
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88">
+        <v>561</v>
+      </c>
+      <c r="E88" t="s">
+        <v>52</v>
+      </c>
+      <c r="F88" s="1">
+        <v>1.8286242093445937</v>
+      </c>
+      <c r="G88" s="1">
+        <v>15553.648796520212</v>
+      </c>
+      <c r="H88" s="1">
+        <v>258845.94762038183</v>
+      </c>
+      <c r="I88" s="1">
+        <v>1076513.4803304502</v>
+      </c>
+      <c r="J88" s="1">
+        <v>4391525.6994513907</v>
+      </c>
+      <c r="K88" s="1">
+        <v>13908504.214614941</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11">
+      <c r="B89" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89" t="s">
+        <v>71</v>
+      </c>
+      <c r="F89" s="1">
+        <v>194.17933650418175</v>
+      </c>
+      <c r="G89" s="1">
+        <v>6371.1092741035509</v>
+      </c>
+      <c r="H89" s="1">
+        <v>31258.272638840761</v>
+      </c>
+      <c r="I89" s="1">
+        <v>75288.355853438858</v>
+      </c>
+      <c r="J89" s="1">
+        <v>211044.54021726499</v>
+      </c>
+      <c r="K89" s="1">
+        <v>542552.43098020181</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11">
+      <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" t="s">
+        <v>17</v>
+      </c>
+      <c r="F90" s="1">
+        <v>409.08169712983124</v>
+      </c>
+      <c r="G90" s="1">
+        <v>1839.315193213268</v>
+      </c>
+      <c r="H90" s="1">
+        <v>15107.496851930342</v>
+      </c>
+      <c r="I90" s="1">
+        <v>53705.550336100336</v>
+      </c>
+      <c r="J90" s="1">
+        <v>276146.76785855967</v>
+      </c>
+      <c r="K90" s="1">
+        <v>1390593.0249165522</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11">
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" s="1">
+        <v>240.51705804576588</v>
+      </c>
+      <c r="G91" s="1">
+        <v>1215.8104555821958</v>
+      </c>
+      <c r="H91" s="1">
+        <v>6248.320419876266</v>
+      </c>
+      <c r="I91" s="1">
+        <v>16368.995601462399</v>
+      </c>
+      <c r="J91" s="1">
+        <v>49562.123258682805</v>
+      </c>
+      <c r="K91" s="1">
+        <v>107967.65500555185</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11">
+      <c r="B92" t="s">
+        <v>81</v>
+      </c>
+      <c r="E92" t="s">
+        <v>72</v>
+      </c>
+      <c r="F92" s="1">
+        <v>826.87801778556229</v>
+      </c>
+      <c r="G92" s="1">
+        <v>6568.6060669587732</v>
+      </c>
+      <c r="H92" s="1">
+        <v>42676.558982756753</v>
+      </c>
+      <c r="I92" s="1">
+        <v>126158.5167588528</v>
+      </c>
+      <c r="J92" s="1">
+        <v>475479.53062918095</v>
+      </c>
+      <c r="K92" s="1">
+        <v>1265026.5051715351</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11">
+      <c r="B93" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" t="s">
+        <v>22</v>
+      </c>
+      <c r="F93" s="1">
+        <v>151.9308797993595</v>
+      </c>
+      <c r="G93" s="1">
+        <v>1502.0924486896611</v>
+      </c>
+      <c r="H93" s="1">
+        <v>9422.6636597741726</v>
+      </c>
+      <c r="I93" s="1">
+        <v>27118.905505335708</v>
+      </c>
+      <c r="J93" s="1">
+        <v>100162.00163572405</v>
+      </c>
+      <c r="K93" s="1">
+        <v>261421.46218751947</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11">
+      <c r="B94" t="s">
+        <v>82</v>
+      </c>
+      <c r="E94" t="s">
+        <v>73</v>
+      </c>
+      <c r="F94" s="1">
+        <v>144.00513388518888</v>
+      </c>
+      <c r="G94" s="1">
+        <v>871.14185517691828</v>
+      </c>
+      <c r="H94" s="1">
+        <v>3857.7689119907677</v>
+      </c>
+      <c r="I94" s="1">
+        <v>8428.2864016885287</v>
+      </c>
+      <c r="J94" s="1">
+        <v>16978.910841784476</v>
+      </c>
+      <c r="K94" s="1">
+        <v>29323.395954775358</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11">
+      <c r="B95" t="s">
+        <v>83</v>
+      </c>
+      <c r="E95" t="s">
+        <v>74</v>
+      </c>
+      <c r="F95" s="1">
+        <v>28.126664630172691</v>
+      </c>
+      <c r="G95" s="1">
+        <v>183.25960593669924</v>
+      </c>
+      <c r="H95" s="1">
+        <v>785.83204702247065</v>
+      </c>
+      <c r="I95" s="1">
+        <v>2025.8877346144275</v>
+      </c>
+      <c r="J95" s="1">
+        <v>7453.3028433327572</v>
+      </c>
+      <c r="K95" s="1">
+        <v>29429.229169638056</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more laser/filter information for lot AJ02
</commit_message>
<xml_diff>
--- a/code/BeadCatalog.xlsx
+++ b/code/BeadCatalog.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="2080" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="1620" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="86">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -274,6 +279,12 @@
   </si>
   <si>
     <t>BUV737</t>
+  </si>
+  <si>
+    <t>PE-Cy5 488</t>
+  </si>
+  <si>
+    <t>PE-Cy5 561</t>
   </si>
 </sst>
 </file>
@@ -286,7 +297,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -624,7 +634,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -634,16 +644,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93:D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -689,7 +699,7 @@
         <v>291016</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -724,7 +734,7 @@
         <v>250485</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -759,7 +769,7 @@
         <v>170258</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -794,7 +804,7 @@
         <v>1069885</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -817,7 +827,7 @@
         <v>503798</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -852,7 +862,7 @@
         <v>146090</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -884,7 +894,7 @@
         <v>26735</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -925,7 +935,7 @@
         <v>293312.93284753093</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -963,7 +973,7 @@
         <v>259412.61657136423</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1011,7 @@
         <v>177982.88390737993</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1049,7 @@
         <v>1120607.1114736947</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>523450.79639630229</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1103,7 +1113,7 @@
         <v>155931.99695048877</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1132,7 +1142,7 @@
         <v>27002.385013650975</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>271771.18947984645</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>251439.20289082278</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1259,7 @@
         <v>188159.82006959253</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1287,7 +1297,7 @@
         <v>1081652.6875898393</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1327,7 @@
         <v>494262.78101307119</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>152052.06356548588</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1385,7 +1395,7 @@
         <v>37257.741435713819</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1426,7 +1436,7 @@
         <v>273002.35313998547</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1464,7 +1474,7 @@
         <v>248049.25900143688</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -1502,7 +1512,7 @@
         <v>179698.3543498595</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1540,7 +1550,7 @@
         <v>1041298.2660207922</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>15</v>
       </c>
@@ -1568,7 +1578,7 @@
         <v>477991.44006706</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -1606,7 +1616,7 @@
         <v>136879.68660749335</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -1644,7 +1654,7 @@
         <v>34373.149263290208</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1682,7 +1692,7 @@
         <v>309755.21324948978</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1717,7 +1727,7 @@
         <v>292771.28196029278</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1752,7 +1762,7 @@
         <v>180682.43671634301</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -1787,7 +1797,7 @@
         <v>830795.86465867609</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1818,7 +1828,7 @@
         <v>133802.14051552708</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1827,7 +1837,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1842,7 +1852,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1874,7 +1884,7 @@
         <v>290986.30857787863</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -1903,7 +1913,7 @@
         <v>250468.6012952716</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -1932,7 +1942,7 @@
         <v>170219.32510029379</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>12</v>
       </c>
@@ -1959,7 +1969,7 @@
         <v>1069920.0890999043</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -1988,7 +1998,7 @@
         <v>147766.14355347541</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2023,7 +2033,7 @@
         <v>319240.8573756913</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -2055,7 +2065,7 @@
         <v>297396.34113562782</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -2087,7 +2097,7 @@
         <v>204118.4615559896</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>12</v>
       </c>
@@ -2119,7 +2129,7 @@
         <v>1308307.6819744271</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>15</v>
       </c>
@@ -2151,7 +2161,7 @@
         <v>474797.25239198504</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>18</v>
       </c>
@@ -2183,7 +2193,7 @@
         <v>199751.06578643262</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>21</v>
       </c>
@@ -2215,7 +2225,7 @@
         <v>40093.000181074385</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="K49" s="2"/>
@@ -2223,7 +2233,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2235,7 +2245,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -2267,7 +2277,7 @@
         <v>18463961</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -2275,7 +2285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>4309984</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -2339,7 +2349,7 @@
         <v>5947886</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>40</v>
       </c>
@@ -2347,7 +2357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2379,7 +2389,7 @@
         <v>328880</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>6</v>
       </c>
@@ -2408,7 +2418,7 @@
         <v>248895</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>12</v>
       </c>
@@ -2437,7 +2447,7 @@
         <v>618430</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>18</v>
       </c>
@@ -2466,7 +2476,7 @@
         <v>919070</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2501,7 +2511,7 @@
         <v>20378.471643026176</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>46</v>
       </c>
@@ -2533,7 +2543,7 @@
         <v>52698.477020820304</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>49</v>
       </c>
@@ -2565,7 +2575,7 @@
         <v>159814.80526382173</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -2597,7 +2607,7 @@
         <v>450950.92072795785</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>6</v>
       </c>
@@ -2629,7 +2639,7 @@
         <v>317887.98611741111</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>9</v>
       </c>
@@ -2661,7 +2671,7 @@
         <v>1187118.7704526538</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>12</v>
       </c>
@@ -2693,7 +2703,7 @@
         <v>1115313.181575086</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>53</v>
       </c>
@@ -2725,7 +2735,7 @@
         <v>536053.21610669303</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>56</v>
       </c>
@@ -2757,7 +2767,7 @@
         <v>51747.05130671752</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>15</v>
       </c>
@@ -2789,7 +2799,7 @@
         <v>1267178.7601849632</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>18</v>
       </c>
@@ -2821,7 +2831,7 @@
         <v>104657.29839566484</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>59</v>
       </c>
@@ -2853,7 +2863,7 @@
         <v>1288085.751604842</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>21</v>
       </c>
@@ -2885,7 +2895,7 @@
         <v>260610.50236340964</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>62</v>
       </c>
@@ -2917,7 +2927,7 @@
         <v>20695.114194178357</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>64</v>
       </c>
@@ -2949,13 +2959,19 @@
         <v>72372.592439871049</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>66</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
       </c>
+      <c r="C77">
+        <v>405</v>
+      </c>
+      <c r="D77" t="s">
+        <v>44</v>
+      </c>
       <c r="E77" t="s">
         <v>45</v>
       </c>
@@ -2978,7 +2994,7 @@
         <v>26699</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>75</v>
       </c>
@@ -3004,10 +3020,16 @@
         <v>66013.697333474352</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>49</v>
       </c>
+      <c r="C79">
+        <v>405</v>
+      </c>
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
       <c r="E79" t="s">
         <v>51</v>
       </c>
@@ -3030,7 +3052,7 @@
         <v>63543.925886697034</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>76</v>
       </c>
@@ -3056,7 +3078,7 @@
         <v>62364.625703974802</v>
       </c>
     </row>
-    <row r="81" spans="2:11">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>77</v>
       </c>
@@ -3082,7 +3104,7 @@
         <v>56753.374460214582</v>
       </c>
     </row>
-    <row r="82" spans="2:11">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>78</v>
       </c>
@@ -3108,10 +3130,16 @@
         <v>56137.007707292629</v>
       </c>
     </row>
-    <row r="83" spans="2:11">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>3</v>
       </c>
+      <c r="C83">
+        <v>488</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
       <c r="E83" t="s">
         <v>5</v>
       </c>
@@ -3134,10 +3162,16 @@
         <v>485705.50301505951</v>
       </c>
     </row>
-    <row r="84" spans="2:11">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>56</v>
       </c>
+      <c r="C84">
+        <v>560</v>
+      </c>
+      <c r="D84" t="s">
+        <v>57</v>
+      </c>
       <c r="E84" t="s">
         <v>58</v>
       </c>
@@ -3160,10 +3194,16 @@
         <v>55123.971224972251</v>
       </c>
     </row>
-    <row r="85" spans="2:11">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>6</v>
       </c>
+      <c r="C85">
+        <v>488</v>
+      </c>
+      <c r="D85" t="s">
+        <v>7</v>
+      </c>
       <c r="E85" t="s">
         <v>8</v>
       </c>
@@ -3186,7 +3226,7 @@
         <v>337422.97853423643</v>
       </c>
     </row>
-    <row r="86" spans="2:11">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>79</v>
       </c>
@@ -3212,12 +3252,15 @@
         <v>1027045.343192119</v>
       </c>
     </row>
-    <row r="87" spans="2:11">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C87">
         <v>488</v>
+      </c>
+      <c r="D87" t="s">
+        <v>13</v>
       </c>
       <c r="E87" t="s">
         <v>52</v>
@@ -3241,9 +3284,9 @@
         <v>1320053.0432920777</v>
       </c>
     </row>
-    <row r="88" spans="2:11">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="C88">
         <v>561</v>
@@ -3270,7 +3313,7 @@
         <v>13908504.214614941</v>
       </c>
     </row>
-    <row r="89" spans="2:11">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>80</v>
       </c>
@@ -3296,10 +3339,16 @@
         <v>542552.43098020181</v>
       </c>
     </row>
-    <row r="90" spans="2:11">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>15</v>
       </c>
+      <c r="C90">
+        <v>488</v>
+      </c>
+      <c r="D90" t="s">
+        <v>16</v>
+      </c>
       <c r="E90" t="s">
         <v>17</v>
       </c>
@@ -3322,10 +3371,16 @@
         <v>1390593.0249165522</v>
       </c>
     </row>
-    <row r="91" spans="2:11">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>18</v>
       </c>
+      <c r="C91">
+        <v>633</v>
+      </c>
+      <c r="D91" t="s">
+        <v>19</v>
+      </c>
       <c r="E91" t="s">
         <v>20</v>
       </c>
@@ -3348,7 +3403,7 @@
         <v>107967.65500555185</v>
       </c>
     </row>
-    <row r="92" spans="2:11">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>81</v>
       </c>
@@ -3374,10 +3429,16 @@
         <v>1265026.5051715351</v>
       </c>
     </row>
-    <row r="93" spans="2:11">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>21</v>
       </c>
+      <c r="C93">
+        <v>635</v>
+      </c>
+      <c r="D93" t="s">
+        <v>16</v>
+      </c>
       <c r="E93" t="s">
         <v>22</v>
       </c>
@@ -3400,7 +3461,7 @@
         <v>261421.46218751947</v>
       </c>
     </row>
-    <row r="94" spans="2:11">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>82</v>
       </c>
@@ -3426,7 +3487,7 @@
         <v>29323.395954775358</v>
       </c>
     </row>
-    <row r="95" spans="2:11">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>83</v>
       </c>
@@ -3455,10 +3516,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remaining URCP lot AJ02 information from SpheroTech
</commit_message>
<xml_diff>
--- a/code/BeadCatalog.xlsx
+++ b/code/BeadCatalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1620" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="800" yWindow="6600" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="90">
   <si>
     <t>SpheroTech RCP-30-5A</t>
   </si>
@@ -272,9 +272,6 @@
     <t>PE-Cy5.5</t>
   </si>
   <si>
-    <t>Alexa 7000</t>
-  </si>
-  <si>
     <t>BUV395</t>
   </si>
   <si>
@@ -285,6 +282,21 @@
   </si>
   <si>
     <t>PE-Cy5 561</t>
+  </si>
+  <si>
+    <t>670/30</t>
+  </si>
+  <si>
+    <t>780/60</t>
+  </si>
+  <si>
+    <t>740/35</t>
+  </si>
+  <si>
+    <t>379/28</t>
+  </si>
+  <si>
+    <t>Alexa 700</t>
   </si>
 </sst>
 </file>
@@ -644,13 +656,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93:D93"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -2998,6 +3011,12 @@
       <c r="B78" t="s">
         <v>75</v>
       </c>
+      <c r="C78">
+        <v>405</v>
+      </c>
+      <c r="D78" t="s">
+        <v>47</v>
+      </c>
       <c r="E78" t="s">
         <v>67</v>
       </c>
@@ -3056,6 +3075,12 @@
       <c r="B80" t="s">
         <v>76</v>
       </c>
+      <c r="C80">
+        <v>405</v>
+      </c>
+      <c r="D80" t="s">
+        <v>85</v>
+      </c>
       <c r="E80" t="s">
         <v>68</v>
       </c>
@@ -3082,6 +3107,12 @@
       <c r="B81" t="s">
         <v>77</v>
       </c>
+      <c r="C81">
+        <v>405</v>
+      </c>
+      <c r="D81" t="s">
+        <v>54</v>
+      </c>
       <c r="E81" t="s">
         <v>69</v>
       </c>
@@ -3108,6 +3139,12 @@
       <c r="B82" t="s">
         <v>78</v>
       </c>
+      <c r="C82">
+        <v>405</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
       <c r="E82" t="s">
         <v>70</v>
       </c>
@@ -3138,7 +3175,7 @@
         <v>488</v>
       </c>
       <c r="D83" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="E83" t="s">
         <v>5</v>
@@ -3167,7 +3204,7 @@
         <v>56</v>
       </c>
       <c r="C84">
-        <v>560</v>
+        <v>488</v>
       </c>
       <c r="D84" t="s">
         <v>57</v>
@@ -3230,6 +3267,12 @@
       <c r="B86" t="s">
         <v>79</v>
       </c>
+      <c r="C86">
+        <v>561</v>
+      </c>
+      <c r="D86" t="s">
+        <v>50</v>
+      </c>
       <c r="E86" t="s">
         <v>11</v>
       </c>
@@ -3254,7 +3297,7 @@
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C87">
         <v>488</v>
@@ -3286,10 +3329,13 @@
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C88">
         <v>561</v>
+      </c>
+      <c r="D88" t="s">
+        <v>85</v>
       </c>
       <c r="E88" t="s">
         <v>52</v>
@@ -3317,6 +3363,12 @@
       <c r="B89" t="s">
         <v>80</v>
       </c>
+      <c r="C89">
+        <v>561</v>
+      </c>
+      <c r="D89" t="s">
+        <v>54</v>
+      </c>
       <c r="E89" t="s">
         <v>71</v>
       </c>
@@ -3344,10 +3396,10 @@
         <v>15</v>
       </c>
       <c r="C90">
-        <v>488</v>
+        <v>561</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="E90" t="s">
         <v>17</v>
@@ -3376,7 +3428,7 @@
         <v>18</v>
       </c>
       <c r="C91">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="D91" t="s">
         <v>19</v>
@@ -3405,7 +3457,13 @@
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>81</v>
+        <v>89</v>
+      </c>
+      <c r="C92">
+        <v>640</v>
+      </c>
+      <c r="D92" t="s">
+        <v>60</v>
       </c>
       <c r="E92" t="s">
         <v>72</v>
@@ -3434,10 +3492,10 @@
         <v>21</v>
       </c>
       <c r="C93">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="D93" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="E93" t="s">
         <v>22</v>
@@ -3463,7 +3521,13 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="C94">
+        <v>355</v>
+      </c>
+      <c r="D94" t="s">
+        <v>88</v>
       </c>
       <c r="E94" t="s">
         <v>73</v>
@@ -3489,7 +3553,13 @@
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="C95">
+        <v>355</v>
+      </c>
+      <c r="D95" t="s">
+        <v>87</v>
       </c>
       <c r="E95" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
added columns to bead catalog
</commit_message>
<xml_diff>
--- a/code/BeadCatalog.xlsx
+++ b/code/BeadCatalog.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/TASBEFlowAnalytics/code/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="800" yWindow="6600" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="1880" yWindow="2020" windowWidth="29180" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -646,7 +641,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -656,17 +651,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58:M95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -712,7 +707,7 @@
         <v>291016</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -747,7 +742,7 @@
         <v>250485</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -782,7 +777,7 @@
         <v>170258</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -817,7 +812,7 @@
         <v>1069885</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -840,7 +835,7 @@
         <v>503798</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -875,7 +870,7 @@
         <v>146090</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -907,7 +902,7 @@
         <v>26735</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -948,7 +943,7 @@
         <v>293312.93284753093</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -986,7 +981,7 @@
         <v>259412.61657136423</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +1019,7 @@
         <v>177982.88390737993</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1057,7 @@
         <v>1120607.1114736947</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1083,7 @@
         <v>523450.79639630229</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1121,7 @@
         <v>155931.99695048877</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1155,7 +1150,7 @@
         <v>27002.385013650975</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1196,7 +1191,7 @@
         <v>271771.18947984645</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1229,7 @@
         <v>251439.20289082278</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -1272,7 +1267,7 @@
         <v>188159.82006959253</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1305,7 @@
         <v>1081652.6875898393</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1340,7 +1335,7 @@
         <v>494262.78101307119</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -1378,7 +1373,7 @@
         <v>152052.06356548588</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1403,7 @@
         <v>37257.741435713819</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1449,7 +1444,7 @@
         <v>273002.35313998547</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>248049.25900143688</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -1525,7 +1520,7 @@
         <v>179698.3543498595</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -1563,7 +1558,7 @@
         <v>1041298.2660207922</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="B27" t="s">
         <v>15</v>
       </c>
@@ -1591,7 +1586,7 @@
         <v>477991.44006706</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -1629,7 +1624,7 @@
         <v>136879.68660749335</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -1667,7 +1662,7 @@
         <v>34373.149263290208</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1705,7 +1700,7 @@
         <v>309755.21324948978</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +1735,7 @@
         <v>292771.28196029278</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>180682.43671634301</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1805,7 @@
         <v>830795.86465867609</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1841,7 +1836,7 @@
         <v>133802.14051552708</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1850,7 +1845,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1865,7 +1860,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1897,7 +1892,7 @@
         <v>290986.30857787863</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1921,7 @@
         <v>250468.6012952716</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -1955,7 +1950,7 @@
         <v>170219.32510029379</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="B40" t="s">
         <v>12</v>
       </c>
@@ -1982,7 +1977,7 @@
         <v>1069920.0890999043</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -2011,7 +2006,7 @@
         <v>147766.14355347541</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2046,7 +2041,7 @@
         <v>319240.8573756913</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -2078,7 +2073,7 @@
         <v>297396.34113562782</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -2110,7 +2105,7 @@
         <v>204118.4615559896</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="B45" t="s">
         <v>12</v>
       </c>
@@ -2142,7 +2137,7 @@
         <v>1308307.6819744271</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="B46" t="s">
         <v>15</v>
       </c>
@@ -2174,7 +2169,7 @@
         <v>474797.25239198504</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="B47" t="s">
         <v>18</v>
       </c>
@@ -2206,7 +2201,7 @@
         <v>199751.06578643262</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="B48" t="s">
         <v>21</v>
       </c>
@@ -2238,7 +2233,7 @@
         <v>40093.000181074385</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14">
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="K49" s="2"/>
@@ -2246,7 +2241,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2258,7 +2253,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -2290,7 +2285,7 @@
         <v>18463961</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -2298,7 +2293,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2330,7 +2325,7 @@
         <v>4309984</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -2362,7 +2357,7 @@
         <v>5947886</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>40</v>
       </c>
@@ -2370,7 +2365,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2401,8 +2396,14 @@
       <c r="K58">
         <v>328880</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="B59" t="s">
         <v>6</v>
       </c>
@@ -2430,8 +2431,14 @@
       <c r="K59">
         <v>248895</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="B60" t="s">
         <v>12</v>
       </c>
@@ -2459,8 +2466,14 @@
       <c r="K60">
         <v>618430</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="B61" t="s">
         <v>18</v>
       </c>
@@ -2488,8 +2501,14 @@
       <c r="K61">
         <v>919070</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2523,8 +2542,14 @@
       <c r="K62" s="3">
         <v>20378.471643026176</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="B63" t="s">
         <v>46</v>
       </c>
@@ -2555,8 +2580,14 @@
       <c r="K63" s="1">
         <v>52698.477020820304</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="B64" t="s">
         <v>49</v>
       </c>
@@ -2587,8 +2618,14 @@
       <c r="K64" s="3">
         <v>159814.80526382173</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="B65" t="s">
         <v>3</v>
       </c>
@@ -2619,8 +2656,14 @@
       <c r="K65" s="3">
         <v>450950.92072795785</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="B66" t="s">
         <v>6</v>
       </c>
@@ -2651,8 +2694,14 @@
       <c r="K66" s="3">
         <v>317887.98611741111</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="B67" t="s">
         <v>9</v>
       </c>
@@ -2683,8 +2732,14 @@
       <c r="K67" s="3">
         <v>1187118.7704526538</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="B68" t="s">
         <v>12</v>
       </c>
@@ -2715,8 +2770,14 @@
       <c r="K68" s="3">
         <v>1115313.181575086</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="B69" t="s">
         <v>53</v>
       </c>
@@ -2747,8 +2808,14 @@
       <c r="K69" s="3">
         <v>536053.21610669303</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="B70" t="s">
         <v>56</v>
       </c>
@@ -2779,8 +2846,14 @@
       <c r="K70" s="3">
         <v>51747.05130671752</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="B71" t="s">
         <v>15</v>
       </c>
@@ -2811,8 +2884,14 @@
       <c r="K71" s="3">
         <v>1267178.7601849632</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="B72" t="s">
         <v>18</v>
       </c>
@@ -2843,8 +2922,14 @@
       <c r="K72" s="3">
         <v>104657.29839566484</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="B73" t="s">
         <v>59</v>
       </c>
@@ -2875,8 +2960,14 @@
       <c r="K73" s="3">
         <v>1288085.751604842</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
       <c r="B74" t="s">
         <v>21</v>
       </c>
@@ -2907,8 +2998,14 @@
       <c r="K74" s="3">
         <v>260610.50236340964</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="B75" t="s">
         <v>62</v>
       </c>
@@ -2939,8 +3036,14 @@
       <c r="K75" s="1">
         <v>20695.114194178357</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
       <c r="B76" t="s">
         <v>64</v>
       </c>
@@ -2971,8 +3074,14 @@
       <c r="K76" s="1">
         <v>72372.592439871049</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>66</v>
       </c>
@@ -3006,8 +3115,14 @@
       <c r="K77" s="3">
         <v>26699</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="B78" t="s">
         <v>75</v>
       </c>
@@ -3038,8 +3153,14 @@
       <c r="K78" s="1">
         <v>66013.697333474352</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
       <c r="B79" t="s">
         <v>49</v>
       </c>
@@ -3070,8 +3191,14 @@
       <c r="K79" s="1">
         <v>63543.925886697034</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="B80" t="s">
         <v>76</v>
       </c>
@@ -3102,8 +3229,14 @@
       <c r="K80" s="1">
         <v>62364.625703974802</v>
       </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13">
       <c r="B81" t="s">
         <v>77</v>
       </c>
@@ -3134,8 +3267,14 @@
       <c r="K81" s="1">
         <v>56753.374460214582</v>
       </c>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13">
       <c r="B82" t="s">
         <v>78</v>
       </c>
@@ -3166,8 +3305,14 @@
       <c r="K82" s="1">
         <v>56137.007707292629</v>
       </c>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13">
       <c r="B83" t="s">
         <v>3</v>
       </c>
@@ -3198,8 +3343,14 @@
       <c r="K83" s="1">
         <v>485705.50301505951</v>
       </c>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13">
       <c r="B84" t="s">
         <v>56</v>
       </c>
@@ -3230,8 +3381,14 @@
       <c r="K84" s="1">
         <v>55123.971224972251</v>
       </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13">
       <c r="B85" t="s">
         <v>6</v>
       </c>
@@ -3262,8 +3419,14 @@
       <c r="K85" s="1">
         <v>337422.97853423643</v>
       </c>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13">
       <c r="B86" t="s">
         <v>79</v>
       </c>
@@ -3294,8 +3457,14 @@
       <c r="K86" s="1">
         <v>1027045.343192119</v>
       </c>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13">
       <c r="B87" t="s">
         <v>83</v>
       </c>
@@ -3326,8 +3495,14 @@
       <c r="K87" s="1">
         <v>1320053.0432920777</v>
       </c>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13">
       <c r="B88" t="s">
         <v>84</v>
       </c>
@@ -3358,8 +3533,14 @@
       <c r="K88" s="1">
         <v>13908504.214614941</v>
       </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13">
       <c r="B89" t="s">
         <v>80</v>
       </c>
@@ -3390,8 +3571,14 @@
       <c r="K89" s="1">
         <v>542552.43098020181</v>
       </c>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13">
       <c r="B90" t="s">
         <v>15</v>
       </c>
@@ -3422,8 +3609,14 @@
       <c r="K90" s="1">
         <v>1390593.0249165522</v>
       </c>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13">
       <c r="B91" t="s">
         <v>18</v>
       </c>
@@ -3454,8 +3647,14 @@
       <c r="K91" s="1">
         <v>107967.65500555185</v>
       </c>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13">
       <c r="B92" t="s">
         <v>89</v>
       </c>
@@ -3486,8 +3685,14 @@
       <c r="K92" s="1">
         <v>1265026.5051715351</v>
       </c>
-    </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13">
       <c r="B93" t="s">
         <v>21</v>
       </c>
@@ -3518,8 +3723,14 @@
       <c r="K93" s="1">
         <v>261421.46218751947</v>
       </c>
-    </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13">
       <c r="B94" t="s">
         <v>81</v>
       </c>
@@ -3550,8 +3761,14 @@
       <c r="K94" s="1">
         <v>29323.395954775358</v>
       </c>
-    </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13">
       <c r="B95" t="s">
         <v>82</v>
       </c>
@@ -3581,10 +3798,21 @@
       </c>
       <c r="K95" s="1">
         <v>29429.229169638056</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>